<commit_message>
new DTWonder PCB files
</commit_message>
<xml_diff>
--- a/boards/dtwonder-DT-R002/BOM.xlsx
+++ b/boards/dtwonder-DT-R002/BOM.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="BOM" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="BOM_ESP32-Wiegand-Hat_ESP32-Wie" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>No.</t>
   </si>
@@ -73,7 +73,7 @@
     <t>2.54-1*8P母环保</t>
   </si>
   <si>
-    <t>Board</t>
+    <t>BOARD</t>
   </si>
   <si>
     <t>HDR-TH_8P-P2.54-V-F-1</t>
@@ -112,7 +112,10 @@
     <t>DP-02RP</t>
   </si>
   <si>
-    <t>DBG</t>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>OFF</t>
   </si>
   <si>
     <t>SW-TH_DP-02XP</t>
@@ -175,7 +178,7 @@
     <t>DB128V-5.08-6P-GN-S</t>
   </si>
   <si>
-    <t>Wiegand</t>
+    <t>WIEGAND</t>
   </si>
   <si>
     <t>CONN-TH_6P-P5.08_DIBO_DB128V-5.08</t>
@@ -561,7 +564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -698,7 +701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -711,155 +714,160 @@
       <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>32</v>
       </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
       <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>